<commit_message>
hong biết đã sửa gì
</commit_message>
<xml_diff>
--- a/Web.ASP/Web.ASP/excel/MauNhapSach.xlsx
+++ b/Web.ASP/Web.ASP/excel/MauNhapSach.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF504C73-14FB-4850-8C7D-06C9BF38F3D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A39B3B-AC8F-4215-871F-120BA1E6DB07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>TG01</t>
   </si>
@@ -154,12 +154,6 @@
   </si>
   <si>
     <t>Meo Meo Meo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size </t>
-  </si>
-  <si>
-    <t>chiều dài x chiều rộng x chiều cao</t>
   </si>
 </sst>
 </file>
@@ -177,7 +171,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,14 +190,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -273,48 +261,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -338,9 +289,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -738,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0277C9-FE35-4581-91FD-0263E6BFA6DA}">
-  <dimension ref="A2:J9"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,7 +699,7 @@
     <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -760,16 +708,8 @@
         <v>28</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="G2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -783,7 +723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -797,7 +737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -811,7 +751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -825,7 +765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -839,7 +779,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -853,7 +793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="12" t="s">

</xml_diff>